<commit_message>
Let's see how she chooches
</commit_message>
<xml_diff>
--- a/Data/UN Population Data/model_values.xlsx
+++ b/Data/UN Population Data/model_values.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="15">
   <si>
     <t>Sweden</t>
   </si>
@@ -559,7 +559,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -590,15 +590,6 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -610,12 +601,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -640,69 +625,87 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="34" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="34" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -986,10 +989,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:U25"/>
+  <dimension ref="A2:AB29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W9" sqref="W9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="Z18" sqref="Z18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,14 +1012,18 @@
     <col min="16" max="16" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.28515625" customWidth="1"/>
+    <col min="19" max="19" width="11.28515625" customWidth="1"/>
+    <col min="20" max="20" width="8.5703125" customWidth="1"/>
+    <col min="21" max="21" width="6.42578125" customWidth="1"/>
+    <col min="22" max="24" width="12.85546875" customWidth="1"/>
+    <col min="25" max="25" width="2.140625" customWidth="1"/>
+    <col min="26" max="28" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="I2" s="42"/>
-    </row>
-    <row r="3" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I2" s="37"/>
+    </row>
+    <row r="3" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1024,27 +1031,39 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="28" t="s">
+      <c r="H3" s="38"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="26"/>
-      <c r="M3" s="24" t="s">
+      <c r="L3" s="23"/>
+      <c r="M3" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="24"/>
+      <c r="N3" s="21"/>
       <c r="O3" s="12"/>
-      <c r="P3" s="18" t="s">
+      <c r="P3" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="19"/>
-      <c r="R3" s="20"/>
-      <c r="S3" s="27"/>
-      <c r="T3" s="27"/>
-    </row>
-    <row r="4" spans="1:21" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q3" s="64"/>
+      <c r="R3" s="65"/>
+      <c r="S3" s="24"/>
+      <c r="T3" s="68"/>
+      <c r="U3" s="68"/>
+      <c r="V3" s="64" t="s">
+        <v>12</v>
+      </c>
+      <c r="W3" s="64"/>
+      <c r="X3" s="65"/>
+      <c r="Y3" s="12"/>
+      <c r="Z3" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA3" s="64"/>
+      <c r="AB3" s="65"/>
+    </row>
+    <row r="4" spans="1:28" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="5" t="s">
         <v>7</v>
@@ -1055,12 +1074,12 @@
       <c r="D4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="43"/>
+      <c r="H4" s="38"/>
       <c r="J4" s="14"/>
-      <c r="K4" s="29"/>
+      <c r="K4" s="67"/>
       <c r="L4" s="13" t="s">
         <v>11</v>
       </c>
@@ -1070,18 +1089,39 @@
       <c r="N4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="36"/>
-      <c r="P4" s="21" t="s">
+      <c r="O4" s="31"/>
+      <c r="P4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="Q4" s="21" t="s">
+      <c r="Q4" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="21" t="s">
+      <c r="R4" s="18" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T4" s="68"/>
+      <c r="U4" s="68"/>
+      <c r="V4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="W4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="X4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y4" s="31"/>
+      <c r="Z4" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA4" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB4" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -1097,10 +1137,10 @@
       <c r="E5" s="7">
         <v>4530426.0000000009</v>
       </c>
-      <c r="I5" s="47" t="s">
+      <c r="I5" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="J5" s="31" t="s">
+      <c r="J5" s="26" t="s">
         <v>4</v>
       </c>
       <c r="K5" s="17">
@@ -1115,8 +1155,8 @@
       <c r="N5" s="17">
         <v>4530426</v>
       </c>
-      <c r="O5" s="37"/>
-      <c r="P5" s="23">
+      <c r="O5" s="32"/>
+      <c r="P5" s="20">
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="Q5" s="17">
@@ -1125,8 +1165,33 @@
       <c r="R5" s="17">
         <v>4487507.0000000009</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T5" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="U5" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="V5" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="W5" s="17">
+        <v>238444</v>
+      </c>
+      <c r="X5" s="17">
+        <v>4530426</v>
+      </c>
+      <c r="Y5" s="32"/>
+      <c r="Z5" s="20">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="AA5" s="17">
+        <v>281363</v>
+      </c>
+      <c r="AB5" s="17">
+        <v>4487507.0000000009</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -1142,71 +1207,119 @@
       <c r="E6" s="7">
         <v>4969722.0000000019</v>
       </c>
-      <c r="I6" s="46"/>
-      <c r="J6" s="52" t="s">
+      <c r="I6" s="60"/>
+      <c r="J6" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="49">
+      <c r="K6" s="40">
         <v>4994695</v>
       </c>
-      <c r="L6" s="51">
+      <c r="L6" s="42">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="M6" s="50">
+      <c r="M6" s="41">
         <v>24973</v>
       </c>
-      <c r="N6" s="49">
+      <c r="N6" s="40">
         <v>4969722</v>
       </c>
-      <c r="O6" s="48"/>
-      <c r="P6" s="53">
+      <c r="O6" s="39"/>
+      <c r="P6" s="44">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="Q6" s="54">
+      <c r="Q6" s="45">
         <v>24973</v>
       </c>
-      <c r="R6" s="55">
+      <c r="R6" s="46">
         <v>4969722.0000000019</v>
       </c>
-      <c r="S6" s="32"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S6" s="27"/>
+      <c r="T6" s="60"/>
+      <c r="U6" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="V6" s="42">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="W6" s="41">
+        <v>24973</v>
+      </c>
+      <c r="X6" s="40">
+        <v>4969722</v>
+      </c>
+      <c r="Y6" s="39"/>
+      <c r="Z6" s="44">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AA6" s="45">
+        <v>24973</v>
+      </c>
+      <c r="AB6" s="46">
+        <v>4969722.0000000019</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
-      <c r="I7" s="44" t="s">
+      <c r="I7" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="34" t="s">
+      <c r="J7" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="K7" s="35">
+      <c r="K7" s="30">
         <v>926285</v>
       </c>
       <c r="L7" s="15">
         <v>0.35</v>
       </c>
-      <c r="M7" s="35">
+      <c r="M7" s="30">
         <v>324200</v>
       </c>
-      <c r="N7" s="38">
+      <c r="N7" s="33">
         <v>602085</v>
       </c>
-      <c r="O7" s="39"/>
-      <c r="P7" s="40">
+      <c r="O7" s="34"/>
+      <c r="P7" s="35">
         <v>0.42899999999999999</v>
       </c>
-      <c r="Q7" s="35">
+      <c r="Q7" s="30">
         <v>397376</v>
       </c>
-      <c r="R7" s="35">
+      <c r="R7" s="30">
         <v>528909</v>
       </c>
-      <c r="S7" s="32"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S7" s="27"/>
+      <c r="T7" s="61" t="s">
+        <v>6</v>
+      </c>
+      <c r="U7" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="V7" s="15">
+        <v>0.35</v>
+      </c>
+      <c r="W7" s="30">
+        <v>324200</v>
+      </c>
+      <c r="X7" s="33">
+        <v>602085</v>
+      </c>
+      <c r="Y7" s="34"/>
+      <c r="Z7" s="35">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="AA7" s="30">
+        <v>397376</v>
+      </c>
+      <c r="AB7" s="30">
+        <v>528909</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -1223,35 +1336,58 @@
         <v>4487507.0000000009</v>
       </c>
       <c r="F8" s="11"/>
-      <c r="I8" s="46"/>
-      <c r="J8" s="59" t="s">
+      <c r="I8" s="60"/>
+      <c r="J8" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="K8" s="49">
+      <c r="K8" s="40">
         <v>1066378</v>
       </c>
-      <c r="L8" s="58">
+      <c r="L8" s="49">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="M8" s="50">
+      <c r="M8" s="41">
         <v>37323</v>
       </c>
-      <c r="N8" s="49">
+      <c r="N8" s="40">
         <v>1029055</v>
       </c>
-      <c r="O8" s="57"/>
-      <c r="P8" s="56">
+      <c r="O8" s="48"/>
+      <c r="P8" s="47">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="Q8" s="50">
+      <c r="Q8" s="41">
         <v>37323</v>
       </c>
-      <c r="R8" s="55">
+      <c r="R8" s="46">
         <v>1029055</v>
       </c>
-      <c r="S8" s="32"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S8" s="27"/>
+      <c r="T8" s="60"/>
+      <c r="U8" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="V8" s="49">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="W8" s="41">
+        <v>37323</v>
+      </c>
+      <c r="X8" s="40">
+        <v>1029055</v>
+      </c>
+      <c r="Y8" s="48"/>
+      <c r="Z8" s="47">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="AA8" s="41">
+        <v>37323</v>
+      </c>
+      <c r="AB8" s="46">
+        <v>1029055</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
@@ -1267,70 +1403,118 @@
       <c r="E9" s="7">
         <v>4969722.0000000019</v>
       </c>
-      <c r="I9" s="44" t="s">
+      <c r="I9" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="J9" s="34" t="s">
+      <c r="J9" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="K9" s="35">
+      <c r="K9" s="30">
         <v>208597</v>
       </c>
       <c r="L9" s="15">
         <v>0.05</v>
       </c>
-      <c r="M9" s="35">
+      <c r="M9" s="30">
         <v>10430</v>
       </c>
-      <c r="N9" s="35">
+      <c r="N9" s="30">
         <v>198167</v>
       </c>
-      <c r="O9" s="39"/>
-      <c r="P9" s="40">
+      <c r="O9" s="34"/>
+      <c r="P9" s="35">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="Q9" s="35">
+      <c r="Q9" s="30">
         <v>20025</v>
       </c>
-      <c r="R9" s="35">
+      <c r="R9" s="30">
         <v>188572</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T9" s="61" t="s">
+        <v>8</v>
+      </c>
+      <c r="U9" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="V9" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="W9" s="30">
+        <v>10430</v>
+      </c>
+      <c r="X9" s="30">
+        <v>198167</v>
+      </c>
+      <c r="Y9" s="34"/>
+      <c r="Z9" s="35">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="AA9" s="30">
+        <v>20025</v>
+      </c>
+      <c r="AB9" s="30">
+        <v>188572</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="60" t="s">
+      <c r="I10" s="62"/>
+      <c r="J10" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="K10" s="61">
+      <c r="K10" s="52">
         <v>219019.00000000003</v>
       </c>
-      <c r="L10" s="62">
+      <c r="L10" s="53">
         <v>3.1E-2</v>
       </c>
-      <c r="M10" s="63">
+      <c r="M10" s="54">
         <v>6790</v>
       </c>
-      <c r="N10" s="65">
+      <c r="N10" s="56">
         <v>212229</v>
       </c>
-      <c r="O10" s="66"/>
-      <c r="P10" s="67">
+      <c r="O10" s="57"/>
+      <c r="P10" s="58">
         <v>3.1E-2</v>
       </c>
-      <c r="Q10" s="63">
+      <c r="Q10" s="54">
         <v>6790</v>
       </c>
-      <c r="R10" s="64">
+      <c r="R10" s="55">
         <v>212229.00000000003</v>
       </c>
-      <c r="S10" s="32"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S10" s="27"/>
+      <c r="T10" s="62"/>
+      <c r="U10" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="V10" s="53">
+        <v>3.1E-2</v>
+      </c>
+      <c r="W10" s="54">
+        <v>6790</v>
+      </c>
+      <c r="X10" s="56">
+        <v>212229</v>
+      </c>
+      <c r="Y10" s="57"/>
+      <c r="Z10" s="58">
+        <v>3.1E-2</v>
+      </c>
+      <c r="AA10" s="54">
+        <v>6790</v>
+      </c>
+      <c r="AB10" s="55">
+        <v>212229.00000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -1339,7 +1523,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
@@ -1352,9 +1536,9 @@
       <c r="E12" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="M12" s="30"/>
-    </row>
-    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M12" s="25"/>
+    </row>
+    <row r="13" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1370,9 +1554,9 @@
       <c r="E13" s="3">
         <v>602085</v>
       </c>
-      <c r="U13" s="41"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U13" s="36"/>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -1389,7 +1573,7 @@
         <v>1029055</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -1521,8 +1705,15 @@
         <v>212229.00000000003</v>
       </c>
     </row>
+    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="11">
+    <mergeCell ref="Z3:AB3"/>
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="T3:U4"/>
+    <mergeCell ref="T5:T6"/>
+    <mergeCell ref="T7:T8"/>
+    <mergeCell ref="T9:T10"/>
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="I9:I10"/>

</xml_diff>